<commit_message>
Progress. So much to fix.
</commit_message>
<xml_diff>
--- a/parameters/parameter_sets.xlsx
+++ b/parameters/parameter_sets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronberliner/MCD/mcd-python/redSun/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronberliner/MCD/mcd-python/redSun/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E92100-9A57-3B4A-813A-8034640D3E68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423742DD-5A4B-D447-8A23-12C00813198D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="2880" windowWidth="38400" windowHeight="21140" xr2:uid="{1D03026E-9647-D54A-961A-F8A9012A15AC}"/>
   </bookViews>
@@ -36,21 +36,12 @@
     <t>parameter</t>
   </si>
   <si>
-    <t>longitude_min</t>
-  </si>
-  <si>
-    <t>longitude_max</t>
-  </si>
-  <si>
     <t>full_value</t>
   </si>
   <si>
     <t>test_value</t>
   </si>
   <si>
-    <t>longitude_step</t>
-  </si>
-  <si>
     <t>sol_min</t>
   </si>
   <si>
@@ -60,24 +51,6 @@
     <t>sol_step</t>
   </si>
   <si>
-    <t>time_min</t>
-  </si>
-  <si>
-    <t>time_max</t>
-  </si>
-  <si>
-    <t>time_step</t>
-  </si>
-  <si>
-    <t>latitude_min</t>
-  </si>
-  <si>
-    <t>latitude_max</t>
-  </si>
-  <si>
-    <t>latitude_step</t>
-  </si>
-  <si>
     <t>half_full_value</t>
   </si>
   <si>
@@ -88,6 +61,33 @@
   </si>
   <si>
     <t>ls_step</t>
+  </si>
+  <si>
+    <t>hr_min</t>
+  </si>
+  <si>
+    <t>hr_max</t>
+  </si>
+  <si>
+    <t>hr_step</t>
+  </si>
+  <si>
+    <t>lat_min</t>
+  </si>
+  <si>
+    <t>lat_max</t>
+  </si>
+  <si>
+    <t>lat_step</t>
+  </si>
+  <si>
+    <t>lon_min</t>
+  </si>
+  <si>
+    <t>lon_max</t>
+  </si>
+  <si>
+    <t>lon_step</t>
   </si>
 </sst>
 </file>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399C6C1B-3F23-BB4F-893D-1BECF6470A95}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,18 +457,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>-90</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>90</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>-180</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>180</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>668</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>24</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>360</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>15</v>

</xml_diff>

<commit_message>
A couple more updates on parameter sets and grid building.
</commit_message>
<xml_diff>
--- a/parameters/parameter_sets.xlsx
+++ b/parameters/parameter_sets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronberliner/MCD/mcd-python/redSun/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426CE1EB-D6E2-7E44-8CE3-7A4413DD1C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C5DE43-DAD2-E54C-B32F-FF450354A302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="2880" windowWidth="38400" windowHeight="21140" xr2:uid="{1D03026E-9647-D54A-961A-F8A9012A15AC}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,7 +653,7 @@
         <v>360</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -664,7 +664,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>